<commit_message>
change species to introduced, add authors
</commit_message>
<xml_diff>
--- a/data_Royal/Royal master species list_version3 FINAL.xlsx
+++ b/data_Royal/Royal master species list_version3 FINAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\PhD\yosemite rnp paper\corrections for 2nd submission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lizzy\Documents\GitHub\wa_inat_plants\data_Royal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96654638-7562-4FE5-90EA-5D8AC1CA2E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C5AFC1-2856-43E9-9000-45354540AC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0B7D541F-466B-4525-A4C7-E6296E71640C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0B7D541F-466B-4525-A4C7-E6296E71640C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -9821,8 +9821,8 @@
   <dimension ref="A1:P1415"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <pane ySplit="1" topLeftCell="A1226" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1173" sqref="F1173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51241,7 +51241,7 @@
         <v>35</v>
       </c>
       <c r="F1172" t="s">
-        <v>12</v>
+        <v>1588</v>
       </c>
       <c r="G1172">
         <v>1</v>

</xml_diff>

<commit_message>
final edits toward Paper 2 submission
</commit_message>
<xml_diff>
--- a/data_Royal/Royal master species list_version3 FINAL.xlsx
+++ b/data_Royal/Royal master species list_version3 FINAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lizzy\Documents\GitHub\wa_inat_plants\data_Royal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C5AFC1-2856-43E9-9000-45354540AC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A726C95-6135-490F-8A76-D01F5E19A2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0B7D541F-466B-4525-A4C7-E6296E71640C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{0B7D541F-466B-4525-A4C7-E6296E71640C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -9821,8 +9821,8 @@
   <dimension ref="A1:P1415"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1226" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1173" sqref="F1173"/>
+      <pane ySplit="1" topLeftCell="A1230" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1283" sqref="F1283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55177,7 +55177,7 @@
         <v>19</v>
       </c>
       <c r="F1283" t="s">
-        <v>12</v>
+        <v>1588</v>
       </c>
       <c r="G1283">
         <v>1</v>

</xml_diff>